<commit_message>
update data driven script
</commit_message>
<xml_diff>
--- a/TestData/testdata.xlsx
+++ b/TestData/testdata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\eclipse-workspace\RestAssured\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48B4359-EA5D-45FE-A494-F954B2D761EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76842DBA-75B3-4390-80C7-E245CDDA01E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0CC6D28C-2C26-45C2-B787-0E8675ADB4AE}"/>
   </bookViews>
@@ -30,37 +30,37 @@
     <t>name</t>
   </si>
   <si>
+    <t>Ryu</t>
+  </si>
+  <si>
+    <t>Ayumi</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
     <t>gender</t>
   </si>
   <si>
     <t>status</t>
   </si>
   <si>
-    <t>Ryu</t>
-  </si>
-  <si>
     <t>male</t>
   </si>
   <si>
     <t>active</t>
   </si>
   <si>
-    <t>Ayumi</t>
-  </si>
-  <si>
     <t>female</t>
   </si>
   <si>
     <t>inactive</t>
   </si>
   <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>ryu.muhammad@gomail.co.id</t>
-  </si>
-  <si>
-    <t>ayumi.kareema@gomail.co.id</t>
+    <t>ryu.muhammad_1@gomail.co.id</t>
+  </si>
+  <si>
+    <t>ayumi.kareema_1@gomail.co.id</t>
   </si>
 </sst>
 </file>
@@ -119,15 +119,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -443,73 +442,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99468C85-015B-4BCD-A2BB-FE11AEC1EFA6}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" customWidth="1"/>
-    <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="1"/>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>6</v>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{A93A3813-534F-4971-99BA-C8EACB9CEB8D}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{C2395F93-28D0-4582-8D90-99D18E2AAE86}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>